<commit_message>
Update - Avec les n°
Tout est dans le titre
</commit_message>
<xml_diff>
--- a/ProjetsRD-Empty.xlsx
+++ b/ProjetsRD-Empty.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="91">
   <si>
     <t xml:space="preserve"> Outils de gestion des absences </t>
   </si>
@@ -285,14 +285,20 @@
     <t>Aupetit</t>
   </si>
   <si>
-    <t>Soiukal</t>
+    <t>N°</t>
+  </si>
+  <si>
+    <t>RESERVE</t>
+  </si>
+  <si>
+    <t>SUPPRIME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,13 +306,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -321,9 +351,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,19 +661,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="107.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -649,8 +693,11 @@
       <c r="F1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -663,8 +710,11 @@
       <c r="D2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -677,8 +727,11 @@
       <c r="D3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -691,8 +744,11 @@
       <c r="D4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -705,8 +761,11 @@
       <c r="D5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -719,8 +778,11 @@
       <c r="D6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -733,8 +795,11 @@
       <c r="D7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -747,8 +812,11 @@
       <c r="D8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -761,8 +829,11 @@
       <c r="D9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -775,8 +846,11 @@
       <c r="D10" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -789,8 +863,11 @@
       <c r="D11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -803,8 +880,11 @@
       <c r="D12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -817,8 +897,11 @@
       <c r="D13" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -831,8 +914,11 @@
       <c r="D14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -845,8 +931,11 @@
       <c r="D15" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -859,8 +948,11 @@
       <c r="D16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="G16" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -873,8 +965,11 @@
       <c r="D17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="G17" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -887,8 +982,11 @@
       <c r="D18" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="G18" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -901,8 +999,11 @@
       <c r="D19" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="G19" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -915,8 +1016,11 @@
       <c r="D20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="G20" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -929,8 +1033,11 @@
       <c r="D21" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="G21" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -943,8 +1050,11 @@
       <c r="D22" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="G22" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -957,8 +1067,11 @@
       <c r="D23" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="G23" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -971,8 +1084,11 @@
       <c r="D24" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="G24" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -985,8 +1101,11 @@
       <c r="D25" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="G25" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -999,8 +1118,11 @@
       <c r="D26" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="G26" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1013,8 +1135,11 @@
       <c r="D27" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="G27" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -1027,8 +1152,11 @@
       <c r="D28" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="G28" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1041,8 +1169,11 @@
       <c r="D29" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="G29" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -1055,8 +1186,11 @@
       <c r="D30" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="G30" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -1069,8 +1203,11 @@
       <c r="D31" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="G31" s="3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -1083,8 +1220,11 @@
       <c r="D32" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="G32" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -1097,8 +1237,11 @@
       <c r="D33" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="G33" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1111,8 +1254,11 @@
       <c r="D34" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="G34" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1125,8 +1271,11 @@
       <c r="D35" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="G35" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1139,8 +1288,11 @@
       <c r="D36" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="G36" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -1153,8 +1305,11 @@
       <c r="D37" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="G37" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -1167,8 +1322,11 @@
       <c r="D38" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="G38" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1181,8 +1339,11 @@
       <c r="D39" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="G39" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1195,8 +1356,11 @@
       <c r="D40" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="G40" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1209,8 +1373,11 @@
       <c r="D41" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="G41" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -1223,8 +1390,11 @@
       <c r="D42" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="G42" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -1237,8 +1407,11 @@
       <c r="D43" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="G43" s="3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1251,8 +1424,11 @@
       <c r="D44" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="G44" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1263,10 +1439,13 @@
         <v>43</v>
       </c>
       <c r="D45" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>86</v>
+      </c>
+      <c r="G45" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -1279,8 +1458,11 @@
       <c r="D46" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="G46" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1293,8 +1475,11 @@
       <c r="D47" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="G47" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1307,8 +1492,11 @@
       <c r="D48" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="G48" s="3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1321,8 +1509,11 @@
       <c r="D49" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="G49" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -1335,8 +1526,11 @@
       <c r="D50" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="G50" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1348,6 +1542,9 @@
       </c>
       <c r="D51" t="s">
         <v>82</v>
+      </c>
+      <c r="G51" s="5">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>